<commit_message>
Funcionalidad del mapa y definicion
</commit_message>
<xml_diff>
--- a/GraficoRutasManagua/src/excel/historial_destinos.xlsx
+++ b/GraficoRutasManagua/src/excel/historial_destinos.xlsx
@@ -443,35 +443,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Multicentro Las Américas</t>
+          <t>Barrio Larreynaga</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Vanegas</t>
+          <t>Ciudad Jardín</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tierra Prometida</t>
+          <t>Barrio San Judas</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Terminal 111</t>
+          <t>Barrio La Primavera</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Camino de Oriente</t>
+          <t>Bello Horizonte</t>
         </is>
       </c>
     </row>

</xml_diff>